<commit_message>
added calcAdjacencies and getTarget and getAdjList and findAllTargets
</commit_message>
<xml_diff>
--- a/data/BoardLayout.xlsx
+++ b/data/BoardLayout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI 306\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI_306\ClueGame\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="29">
   <si>
     <t>C</t>
   </si>
@@ -91,6 +91,27 @@
   <si>
     <t>W</t>
   </si>
+  <si>
+    <t>White: door direction tests (in BoardInitTests)</t>
+  </si>
+  <si>
+    <t>Orange: adjacency list tests, inside rooms</t>
+  </si>
+  <si>
+    <t>Purple: adjacency list tests, room exits</t>
+  </si>
+  <si>
+    <t>Green:adjacency lists beide room entrance</t>
+  </si>
+  <si>
+    <t>Light Blue: test targets</t>
+  </si>
+  <si>
+    <t>Number of Doors: 14</t>
+  </si>
+  <si>
+    <t>Light Pink: walkway scenarios</t>
+  </si>
 </sst>
 </file>
 
@@ -119,7 +140,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,6 +183,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -175,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -184,6 +235,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -192,6 +249,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF99FF"/>
+      <color rgb="FFCC00FF"/>
       <color rgb="FFFF0000"/>
     </mruColors>
   </colors>
@@ -469,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA27"/>
+  <dimension ref="A1:AA35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AG21" sqref="AG21"/>
+      <selection activeCell="AD15" sqref="AD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,7 +564,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -580,7 +639,7 @@
       <c r="Y1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="10" t="s">
         <v>4</v>
       </c>
       <c r="AA1" s="7">
@@ -716,7 +775,7 @@
       <c r="O3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="8" t="s">
         <v>20</v>
       </c>
       <c r="Q3" s="2" t="s">
@@ -763,7 +822,7 @@
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="8" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -858,7 +917,7 @@
       <c r="G5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I5" s="4" t="s">
@@ -885,13 +944,13 @@
       <c r="P5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Q5" s="2" t="s">
+      <c r="Q5" s="11" t="s">
         <v>21</v>
       </c>
       <c r="R5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S5" s="2" t="s">
+      <c r="S5" s="13" t="s">
         <v>21</v>
       </c>
       <c r="T5" s="2" t="s">
@@ -989,7 +1048,7 @@
       <c r="W6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="X6" s="3" t="s">
+      <c r="X6" s="13" t="s">
         <v>13</v>
       </c>
       <c r="Y6" s="4" t="s">
@@ -1012,7 +1071,7 @@
       <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="12" t="s">
         <v>21</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -1072,7 +1131,7 @@
       <c r="W7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="X7" s="2" t="s">
+      <c r="X7" s="11" t="s">
         <v>21</v>
       </c>
       <c r="Y7" s="2" t="s">
@@ -1086,7 +1145,7 @@
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1676,7 +1735,7 @@
       <c r="C15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="13" t="s">
         <v>16</v>
       </c>
       <c r="E15" s="2" t="s">
@@ -1733,7 +1792,7 @@
       <c r="V15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W15" s="2" t="s">
+      <c r="W15" s="13" t="s">
         <v>21</v>
       </c>
       <c r="X15" s="2" t="s">
@@ -1866,7 +1925,7 @@
       <c r="K17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="L17" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M17" s="2" t="s">
@@ -1890,7 +1949,7 @@
       <c r="S17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="T17" s="3" t="s">
+      <c r="T17" s="8" t="s">
         <v>12</v>
       </c>
       <c r="U17" s="4" t="s">
@@ -1928,7 +1987,7 @@
       <c r="D18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="13" t="s">
         <v>21</v>
       </c>
       <c r="F18" s="2" t="s">
@@ -1955,7 +2014,7 @@
       <c r="M18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N18" s="2" t="s">
+      <c r="N18" s="11" t="s">
         <v>21</v>
       </c>
       <c r="O18" s="2" t="s">
@@ -2106,7 +2165,7 @@
       <c r="H20" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="I20" s="13" t="s">
         <v>21</v>
       </c>
       <c r="J20" s="2" t="s">
@@ -2136,7 +2195,7 @@
       <c r="R20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S20" s="2" t="s">
+      <c r="S20" s="12" t="s">
         <v>21</v>
       </c>
       <c r="T20" s="4" t="s">
@@ -2248,7 +2307,7 @@
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="13" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -2302,7 +2361,7 @@
       <c r="R22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S22" s="2" t="s">
+      <c r="S22" s="11" t="s">
         <v>21</v>
       </c>
       <c r="T22" s="3" t="s">
@@ -2655,7 +2714,7 @@
       <c r="Y26" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="Z26" s="4" t="s">
+      <c r="Z26" s="10" t="s">
         <v>5</v>
       </c>
       <c r="AA26" s="7">
@@ -2740,6 +2799,41 @@
       </c>
       <c r="Z27" s="7">
         <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Current state: failing tests
</commit_message>
<xml_diff>
--- a/data/BoardLayout.xlsx
+++ b/data/BoardLayout.xlsx
@@ -140,7 +140,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,13 +203,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -226,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -238,9 +244,10 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,7 +538,7 @@
   <dimension ref="A1:AA35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AD15" sqref="AD15"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +571,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -600,7 +607,7 @@
       <c r="L1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="12" t="s">
         <v>21</v>
       </c>
       <c r="N1" s="4" t="s">
@@ -639,7 +646,7 @@
       <c r="Y1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="Z1" s="10" t="s">
+      <c r="Z1" s="13" t="s">
         <v>4</v>
       </c>
       <c r="AA1" s="7">
@@ -858,7 +865,7 @@
       <c r="O4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="P4" s="14" t="s">
         <v>20</v>
       </c>
       <c r="Q4" s="2" t="s">
@@ -911,7 +918,7 @@
       <c r="E5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="12" t="s">
         <v>21</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -926,7 +933,7 @@
       <c r="J5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="12" t="s">
         <v>18</v>
       </c>
       <c r="L5" s="2" t="s">
@@ -944,19 +951,19 @@
       <c r="P5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Q5" s="11" t="s">
+      <c r="Q5" s="10" t="s">
         <v>21</v>
       </c>
       <c r="R5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S5" s="13" t="s">
+      <c r="S5" s="12" t="s">
         <v>21</v>
       </c>
       <c r="T5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="U5" s="2" t="s">
+      <c r="U5" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V5" s="4" t="s">
@@ -982,7 +989,7 @@
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1048,7 +1055,7 @@
       <c r="W6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="X6" s="13" t="s">
+      <c r="X6" s="12" t="s">
         <v>13</v>
       </c>
       <c r="Y6" s="4" t="s">
@@ -1071,13 +1078,13 @@
       <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>21</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="12" t="s">
         <v>21</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -1131,7 +1138,7 @@
       <c r="W7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="X7" s="11" t="s">
+      <c r="X7" s="10" t="s">
         <v>21</v>
       </c>
       <c r="Y7" s="2" t="s">
@@ -1466,7 +1473,7 @@
       <c r="X11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="Y11" s="2" t="s">
+      <c r="Y11" s="11" t="s">
         <v>21</v>
       </c>
       <c r="Z11" s="2" t="s">
@@ -1735,7 +1742,7 @@
       <c r="C15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>16</v>
       </c>
       <c r="E15" s="2" t="s">
@@ -1792,7 +1799,7 @@
       <c r="V15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W15" s="13" t="s">
+      <c r="W15" s="2" t="s">
         <v>21</v>
       </c>
       <c r="X15" s="2" t="s">
@@ -1925,7 +1932,7 @@
       <c r="K17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L17" s="13" t="s">
+      <c r="L17" s="12" t="s">
         <v>21</v>
       </c>
       <c r="M17" s="2" t="s">
@@ -1987,7 +1994,7 @@
       <c r="D18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="12" t="s">
         <v>21</v>
       </c>
       <c r="F18" s="2" t="s">
@@ -2014,7 +2021,7 @@
       <c r="M18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N18" s="11" t="s">
+      <c r="N18" s="10" t="s">
         <v>21</v>
       </c>
       <c r="O18" s="2" t="s">
@@ -2061,7 +2068,7 @@
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -2165,7 +2172,7 @@
       <c r="H20" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="13" t="s">
+      <c r="I20" s="12" t="s">
         <v>21</v>
       </c>
       <c r="J20" s="2" t="s">
@@ -2195,7 +2202,7 @@
       <c r="R20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S20" s="12" t="s">
+      <c r="S20" s="11" t="s">
         <v>21</v>
       </c>
       <c r="T20" s="4" t="s">
@@ -2307,7 +2314,7 @@
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -2361,7 +2368,7 @@
       <c r="R22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S22" s="11" t="s">
+      <c r="S22" s="10" t="s">
         <v>21</v>
       </c>
       <c r="T22" s="3" t="s">
@@ -2429,7 +2436,7 @@
       <c r="M23" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N23" s="4" t="s">
+      <c r="N23" s="13" t="s">
         <v>6</v>
       </c>
       <c r="O23" s="4" t="s">
@@ -2473,7 +2480,7 @@
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -2485,7 +2492,7 @@
       <c r="D24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="13" t="s">
         <v>10</v>
       </c>
       <c r="F24" s="1" t="s">
@@ -2666,7 +2673,7 @@
       <c r="I26" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="J26" s="11" t="s">
         <v>21</v>
       </c>
       <c r="K26" s="2" t="s">
@@ -2714,7 +2721,7 @@
       <c r="Y26" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="Z26" s="10" t="s">
+      <c r="Z26" s="13" t="s">
         <v>5</v>
       </c>
       <c r="AA26" s="7">

</xml_diff>

<commit_message>
Fixed calcAdjacencies to account for doorway directins, fixed all tests to pass
</commit_message>
<xml_diff>
--- a/data/BoardLayout.xlsx
+++ b/data/BoardLayout.xlsx
@@ -538,7 +538,7 @@
   <dimension ref="A1:AA35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1816,7 +1816,7 @@
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1891,7 +1891,7 @@
       <c r="Y16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Z16" s="2" t="s">
+      <c r="Z16" s="12" t="s">
         <v>21</v>
       </c>
       <c r="AA16" s="7">
@@ -1994,7 +1994,7 @@
       <c r="D18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F18" s="2" t="s">
@@ -2655,7 +2655,7 @@
       <c r="C26" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="12" t="s">
         <v>21</v>
       </c>
       <c r="E26" s="1" t="s">
@@ -2694,7 +2694,7 @@
       <c r="P26" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="Q26" s="2" t="s">
+      <c r="Q26" s="12" t="s">
         <v>21</v>
       </c>
       <c r="R26" s="2" t="s">

</xml_diff>